<commit_message>
e2e perf app, docs, and results (#28)
</commit_message>
<xml_diff>
--- a/otelcollector/perf/OtelCollectorScaleTesting.xlsx
+++ b/otelcollector/perf/OtelCollectorScaleTesting.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24123"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EA2ACAE-F230-4B13-ADD9-3DD10C98B04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EEEF8A9-F3D3-4D47-A433-22D276DD342F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="04-26-21" sheetId="1" r:id="rId1"/>
     <sheet name="04-30-21" sheetId="2" r:id="rId2"/>
+    <sheet name="5-20-21" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="48">
   <si>
     <t>Node: DS3v2      4 cores, 14 GiB</t>
   </si>
@@ -95,9 +96,6 @@
     <t># of Instances</t>
   </si>
   <si>
-    <t>Batch Size</t>
-  </si>
-  <si>
     <t>Total Timeseries</t>
   </si>
   <si>
@@ -131,10 +129,49 @@
     <t>15m</t>
   </si>
   <si>
-    <t>Richi: 1,295,069 active series @ 15 second scrape interval with 1.3-1.6 cores = 59,543.40 samples/second/core</t>
-  </si>
-  <si>
-    <t>Jaana: 15s scraping frequency only became a bottleneck when 1000 metrics are exported from 50+ replicas</t>
+    <t>15s Interval</t>
+  </si>
+  <si>
+    <t>DS4v2 Node</t>
+  </si>
+  <si>
+    <t>Targets</t>
+  </si>
+  <si>
+    <t>Metric Count</t>
+  </si>
+  <si>
+    <t>Timeseries Count</t>
+  </si>
+  <si>
+    <t>CPU (cores)</t>
+  </si>
+  <si>
+    <t>RAM (GiB)</t>
+  </si>
+  <si>
+    <t>Max Batch Metrics Size</t>
+  </si>
+  <si>
+    <t>Timeseries</t>
+  </si>
+  <si>
+    <t>Labels</t>
+  </si>
+  <si>
+    <t>62,500 each</t>
+  </si>
+  <si>
+    <t>500,000 each</t>
+  </si>
+  <si>
+    <t>DS3v2 Node</t>
+  </si>
+  <si>
+    <t>Max Batch Size for a single scrape</t>
+  </si>
+  <si>
+    <t>E2E Scale Testing</t>
   </si>
 </sst>
 </file>
@@ -210,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -281,14 +318,54 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="28">
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
@@ -481,55 +558,80 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A0519C5-FC89-427E-959A-0CB0268EF96D}" name="Table1" displayName="Table1" ref="B4:N50" totalsRowShown="0" headerRowDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A0519C5-FC89-427E-959A-0CB0268EF96D}" name="Table1" displayName="Table1" ref="B4:N50" totalsRowShown="0" headerRowDxfId="27">
   <autoFilter ref="B4:N50" xr:uid="{5A0519C5-FC89-427E-959A-0CB0268EF96D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:N50">
     <sortCondition descending="1" ref="N4:N50"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{BF2CDB35-8AC5-4AEA-BA22-5C4D024916A8}" name="Instances" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{12ECEACB-5005-40C2-B3D5-FB499000FF84}" name="Duration (m)" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{291AE65D-D972-4B2B-8320-18B905551432}" name="Scrape Interval (s)" dataDxfId="19"/>
-    <tableColumn id="14" xr3:uid="{0126D56C-9783-47D9-8C08-0BC977845579}" name="Data Points / Metric" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{3EBF7F41-5C1E-454C-BFFF-212FE8ABDA6F}" name="Items Sent" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{4C7CF128-6ED0-4FFF-AFF7-1F5BED757A37}" name="Items / Second" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{BF2CDB35-8AC5-4AEA-BA22-5C4D024916A8}" name="Instances" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{12ECEACB-5005-40C2-B3D5-FB499000FF84}" name="Duration (m)" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{291AE65D-D972-4B2B-8320-18B905551432}" name="Scrape Interval (s)" dataDxfId="24"/>
+    <tableColumn id="14" xr3:uid="{0126D56C-9783-47D9-8C08-0BC977845579}" name="Data Points / Metric" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{3EBF7F41-5C1E-454C-BFFF-212FE8ABDA6F}" name="Items Sent" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{4C7CF128-6ED0-4FFF-AFF7-1F5BED757A37}" name="Items / Second" dataDxfId="21">
       <calculatedColumnFormula>F5/(C5*60)*B5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{6109DA89-2E0D-4201-B62A-8AE5331831B2}" name="Avg CPU %" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{C9CBC5E4-EF2B-4343-8C92-4747149FD949}" name="Max CPU %" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{1DF99B1E-9956-4BA7-AB2A-7CD154F271A1}" name="RAM Avg MiB" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{6E9FAC7A-49EC-44A4-ACC4-53F2587FCAD8}" name="RAM Max MiB" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{BE64B27B-CE16-4997-91DE-FD07EFA423B2}" name="Items Scraped" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{CEFD4538-B82A-4290-A6ED-A960A4EC02D9}" name="Pass/Fail" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{2199900F-5C8A-4988-B841-8FA3583BE260}" name="Time Diff = Interval?" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{6109DA89-2E0D-4201-B62A-8AE5331831B2}" name="Avg CPU %" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{C9CBC5E4-EF2B-4343-8C92-4747149FD949}" name="Max CPU %" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{1DF99B1E-9956-4BA7-AB2A-7CD154F271A1}" name="RAM Avg MiB" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{6E9FAC7A-49EC-44A4-ACC4-53F2587FCAD8}" name="RAM Max MiB" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{BE64B27B-CE16-4997-91DE-FD07EFA423B2}" name="Items Scraped" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{CEFD4538-B82A-4290-A6ED-A960A4EC02D9}" name="Pass/Fail" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{2199900F-5C8A-4988-B841-8FA3583BE260}" name="Time Diff = Interval?" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A22B299E-A0B8-47B3-A3B1-B6A71CF80539}" name="Table2" displayName="Table2" ref="B2:O10" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="B2:O10" xr:uid="{A22B299E-A0B8-47B3-A3B1-B6A71CF80539}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:O9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A22B299E-A0B8-47B3-A3B1-B6A71CF80539}" name="Table2" displayName="Table2" ref="B2:N10" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="B2:N10" xr:uid="{A22B299E-A0B8-47B3-A3B1-B6A71CF80539}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:N9">
     <sortCondition ref="D2:D9"/>
   </sortState>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{CE775671-A2AA-4385-B468-3C70ED9E8979}" name="Duration" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{EA83BEBB-8A08-4815-87FE-103B51E15934}" name="Scrape Interval" dataDxfId="6"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{CE775671-A2AA-4385-B468-3C70ED9E8979}" name="Duration" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{EA83BEBB-8A08-4815-87FE-103B51E15934}" name="Scrape Interval" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{1E2887D9-C9A3-4B46-801B-2C49E7C10299}" name="# of Instances"/>
-    <tableColumn id="14" xr3:uid="{88422D2C-134D-41A3-83FE-E57B9A85E7DC}" name="Batch Size">
-      <calculatedColumnFormula>5000*7</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{8A93E72F-B6BB-423C-8E01-876B58068CD1}" name="Total Timeseries" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{1C975E3A-6C49-4BD5-8E47-4F1691316A20}" name="Timeseries / Instance" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{C9516E2D-1C32-4AED-8DB7-68761C44DE2B}" name="Samples / Sec" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{8A93E72F-B6BB-423C-8E01-876B58068CD1}" name="Total Timeseries" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{1C975E3A-6C49-4BD5-8E47-4F1691316A20}" name="Timeseries / Instance" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{C9516E2D-1C32-4AED-8DB7-68761C44DE2B}" name="Samples / Sec" dataDxfId="8"/>
     <tableColumn id="7" xr3:uid="{2E75DA5B-E153-4733-B79E-3D9C2563C431}" name="CPU Avg %"/>
     <tableColumn id="8" xr3:uid="{3C339738-6966-409E-A445-28D04D4B7EC1}" name="CPU Max %"/>
     <tableColumn id="9" xr3:uid="{86C77617-868E-430F-9E05-0C724A3062B2}" name="RAM Avg MiB"/>
     <tableColumn id="10" xr3:uid="{74E8E469-6B3D-4973-B0CA-1E9ECD96A95D}" name="RAM Max MiB"/>
-    <tableColumn id="11" xr3:uid="{67A3BDCD-6553-41CB-B951-0A60CC8905D7}" name="Samples / Sec / Core (Avg)" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{7C55408E-1426-46FE-8CD1-2B1A74A29A30}" name="Samples / Sec  / Core (Max)" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{60C0139A-8D82-44E9-BA37-13B989764AED}" name="Samples / Sec / Instance" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{67A3BDCD-6553-41CB-B951-0A60CC8905D7}" name="Samples / Sec / Core (Avg)" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{7C55408E-1426-46FE-8CD1-2B1A74A29A30}" name="Samples / Sec  / Core (Max)" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{60C0139A-8D82-44E9-BA37-13B989764AED}" name="Samples / Sec / Instance" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A4E90DDC-778C-4ABE-B7BD-AF40BEFC7B7A}" name="Table3" displayName="Table3" ref="B2:G6" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="B2:G6" xr:uid="{A4E90DDC-778C-4ABE-B7BD-AF40BEFC7B7A}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{510BE4D4-628B-4B7C-B1EC-787030378EED}" name="Targets"/>
+    <tableColumn id="2" xr3:uid="{4AE9FA2C-921B-4EFA-94EF-5CF0A900B150}" name="Scrape Interval"/>
+    <tableColumn id="3" xr3:uid="{2F0DD86E-529F-496E-9922-2D0879EE5931}" name="Metric Count" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{7FA782B8-C59D-4670-9D9A-FB7A01D8B00D}" name="Timeseries Count" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{096BEF50-736C-4740-A1DD-A66D38AB7068}" name="CPU (cores)"/>
+    <tableColumn id="6" xr3:uid="{F7050663-9F58-4C26-8E59-FCCD5CBE16E3}" name="RAM (GiB)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{42883285-A6A2-4411-BF4F-13E87625C319}" name="Table4" displayName="Table4" ref="I2:L7" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="I2:L7" xr:uid="{42883285-A6A2-4411-BF4F-13E87625C319}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{CD591FBC-7835-4462-9E35-5D5FC44D26DD}" name="Max Batch Metrics Size"/>
+    <tableColumn id="2" xr3:uid="{4423BCAF-E816-4EC8-9433-812CCDC5EB38}" name="Timeseries"/>
+    <tableColumn id="3" xr3:uid="{B7F491EC-0CED-43DF-BD55-464F7C2791C0}" name="Labels"/>
+    <tableColumn id="4" xr3:uid="{8D1505F4-3CCD-4081-A1A7-54DF605E6F6C}" name="Total Timeseries" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -834,7 +936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:T53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O57" sqref="O57"/>
     </sheetView>
   </sheetViews>
@@ -2872,31 +2974,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{522B4482-97C4-40B2-972B-E16F54B4F931}">
-  <dimension ref="B2:O13"/>
+  <dimension ref="B2:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="22" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" style="22" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="17" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" style="22" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" style="22" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" s="24" customFormat="1" ht="30" customHeight="1">
+    <row r="2" spans="2:14" s="24" customFormat="1" ht="30" customHeight="1">
       <c r="B2" s="23" t="s">
         <v>19</v>
       </c>
@@ -2906,7 +3007,7 @@
       <c r="D2" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="23" t="s">
         <v>22</v>
       </c>
       <c r="F2" s="23" t="s">
@@ -2922,13 +3023,13 @@
         <v>26</v>
       </c>
       <c r="J2" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="25" t="s">
         <v>27</v>
-      </c>
-      <c r="K2" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="23" t="s">
-        <v>11</v>
       </c>
       <c r="M2" s="25" t="s">
         <v>28</v>
@@ -2936,406 +3037,593 @@
       <c r="N2" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="25" t="s">
+    </row>
+    <row r="3" spans="2:14">
+      <c r="B3" s="21" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="2:15">
-      <c r="B3" s="21" t="s">
+      <c r="C3" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>32</v>
-      </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <f>5000*7</f>
-        <v>35000</v>
+      <c r="E3" s="22">
+        <v>1000000</v>
       </c>
       <c r="F3" s="22">
         <v>1000000</v>
       </c>
       <c r="G3" s="22">
+        <v>66666</v>
+      </c>
+      <c r="H3">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="I3">
+        <v>232.3</v>
+      </c>
+      <c r="J3">
+        <v>2896</v>
+      </c>
+      <c r="K3">
+        <v>3028</v>
+      </c>
+      <c r="L3" s="22">
+        <f>G3/(H3/100)</f>
+        <v>87259.162303664925</v>
+      </c>
+      <c r="M3" s="22">
+        <f>G3/(I3/100)</f>
+        <v>28698.235040895393</v>
+      </c>
+      <c r="N3" s="22">
+        <f>G3/D3</f>
+        <v>66666</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14">
+      <c r="B4" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="22">
         <v>1000000</v>
-      </c>
-      <c r="H3" s="22">
-        <v>66666</v>
-      </c>
-      <c r="I3">
-        <v>76.400000000000006</v>
-      </c>
-      <c r="J3">
-        <v>232.3</v>
-      </c>
-      <c r="K3">
-        <v>2896</v>
-      </c>
-      <c r="L3">
-        <v>3028</v>
-      </c>
-      <c r="M3" s="22">
-        <f>H3/(I3/100)</f>
-        <v>87259.162303664925</v>
-      </c>
-      <c r="N3" s="22">
-        <f>H3/(J3/100)</f>
-        <v>28698.235040895393</v>
-      </c>
-      <c r="O3" s="22">
-        <f>H3/D3</f>
-        <v>66666</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15">
-      <c r="B4" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E10" si="0">5000*7</f>
-        <v>35000</v>
       </c>
       <c r="F4" s="22">
         <v>1000000</v>
       </c>
       <c r="G4" s="22">
+        <v>66666</v>
+      </c>
+      <c r="H4">
+        <v>71.2</v>
+      </c>
+      <c r="I4">
+        <v>218.3</v>
+      </c>
+      <c r="J4">
+        <v>2468</v>
+      </c>
+      <c r="K4">
+        <v>2791</v>
+      </c>
+      <c r="L4" s="22">
+        <f>G4/(H4/100)</f>
+        <v>93632.022471910095</v>
+      </c>
+      <c r="M4" s="22">
+        <f>G4/(I4/100)</f>
+        <v>30538.708199725144</v>
+      </c>
+      <c r="N4" s="22">
+        <f>G4/D4</f>
+        <v>66666</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" hidden="1">
+      <c r="B5" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="22">
         <v>1000000</v>
-      </c>
-      <c r="H4" s="22">
-        <v>66666</v>
-      </c>
-      <c r="I4">
-        <v>71.2</v>
-      </c>
-      <c r="J4">
-        <v>218.3</v>
-      </c>
-      <c r="K4">
-        <v>2468</v>
-      </c>
-      <c r="L4">
-        <v>2791</v>
-      </c>
-      <c r="M4" s="22">
-        <f>H4/(I4/100)</f>
-        <v>93632.022471910095</v>
-      </c>
-      <c r="N4" s="22">
-        <f>H4/(J4/100)</f>
-        <v>30538.708199725144</v>
-      </c>
-      <c r="O4" s="22">
-        <f>H4/D4</f>
-        <v>66666</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" hidden="1">
-      <c r="B5" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1000</v>
       </c>
       <c r="F5" s="22">
         <v>1000000</v>
       </c>
       <c r="G5" s="22">
+        <v>66666</v>
+      </c>
+      <c r="H5">
+        <v>67.3</v>
+      </c>
+      <c r="I5">
+        <v>220</v>
+      </c>
+      <c r="J5">
+        <v>2368</v>
+      </c>
+      <c r="K5">
+        <v>2583</v>
+      </c>
+      <c r="L5" s="22">
+        <f>G5/(H5/100)</f>
+        <v>99057.94947994058</v>
+      </c>
+      <c r="M5" s="22">
+        <f>G5/(I5/100)</f>
+        <v>30302.727272727272</v>
+      </c>
+      <c r="N5" s="22">
+        <f>G5/D5</f>
+        <v>66666</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14">
+      <c r="B6" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="22">
         <v>1000000</v>
       </c>
-      <c r="H5" s="22">
+      <c r="F6" s="22">
+        <v>500000</v>
+      </c>
+      <c r="G6" s="22">
         <v>66666</v>
       </c>
-      <c r="I5">
-        <v>67.3</v>
-      </c>
-      <c r="J5">
-        <v>220</v>
-      </c>
-      <c r="K5">
-        <v>2368</v>
-      </c>
-      <c r="L5">
-        <v>2583</v>
-      </c>
-      <c r="M5" s="22">
-        <f>H5/(I5/100)</f>
-        <v>99057.94947994058</v>
-      </c>
-      <c r="N5" s="22">
-        <f>H5/(J5/100)</f>
-        <v>30302.727272727272</v>
-      </c>
-      <c r="O5" s="22">
-        <f>H5/D5</f>
-        <v>66666</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15">
-      <c r="B6" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="21" t="s">
+      <c r="H6">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="I6">
+        <v>201</v>
+      </c>
+      <c r="J6">
+        <v>1772</v>
+      </c>
+      <c r="K6">
+        <v>1885</v>
+      </c>
+      <c r="L6" s="22">
+        <f>G6/(H6/100)</f>
+        <v>93108.938547486032</v>
+      </c>
+      <c r="M6" s="22">
+        <f>G6/(I6/100)</f>
+        <v>33167.164179104482</v>
+      </c>
+      <c r="N6" s="22">
+        <f>G6/D6</f>
+        <v>33333</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14">
+      <c r="B7" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>35000</v>
-      </c>
-      <c r="F6" s="22">
-        <v>1000000</v>
-      </c>
-      <c r="G6" s="22">
-        <v>500000</v>
-      </c>
-      <c r="H6" s="22">
-        <v>66666</v>
-      </c>
-      <c r="I6">
-        <v>71.599999999999994</v>
-      </c>
-      <c r="J6">
-        <v>201</v>
-      </c>
-      <c r="K6">
-        <v>1772</v>
-      </c>
-      <c r="L6">
-        <v>1885</v>
-      </c>
-      <c r="M6" s="22">
-        <f>H6/(I6/100)</f>
-        <v>93108.938547486032</v>
-      </c>
-      <c r="N6" s="22">
-        <f>H6/(J6/100)</f>
-        <v>33167.164179104482</v>
-      </c>
-      <c r="O6" s="22">
-        <f>H6/D6</f>
-        <v>33333</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15">
-      <c r="B7" s="21" t="s">
-        <v>33</v>
-      </c>
       <c r="C7" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>35000</v>
+      <c r="E7" s="22">
+        <v>1000000</v>
       </c>
       <c r="F7" s="22">
-        <v>1000000</v>
+        <v>333333</v>
       </c>
       <c r="G7" s="22">
-        <v>333333</v>
-      </c>
-      <c r="H7" s="22">
         <v>66666</v>
       </c>
+      <c r="H7">
+        <v>74.400000000000006</v>
+      </c>
       <c r="I7">
-        <v>74.400000000000006</v>
+        <v>174</v>
       </c>
       <c r="J7">
-        <v>174</v>
+        <v>1611</v>
       </c>
       <c r="K7">
-        <v>1611</v>
-      </c>
-      <c r="L7">
         <v>1725</v>
       </c>
+      <c r="L7" s="22">
+        <f>G7/(H7/100)</f>
+        <v>89604.838709677409</v>
+      </c>
       <c r="M7" s="22">
-        <f>H7/(I7/100)</f>
-        <v>89604.838709677409</v>
+        <f>G7/(I7/100)</f>
+        <v>38313.793103448275</v>
       </c>
       <c r="N7" s="22">
-        <f>H7/(J7/100)</f>
-        <v>38313.793103448275</v>
-      </c>
-      <c r="O7" s="22">
-        <f>H7/D7</f>
+        <f>G7/D7</f>
         <v>22222</v>
       </c>
     </row>
-    <row r="8" spans="2:15">
+    <row r="8" spans="2:14">
       <c r="B8" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8">
         <v>4</v>
       </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>35000</v>
+      <c r="E8" s="22">
+        <v>1000000</v>
       </c>
       <c r="F8" s="22">
-        <v>1000000</v>
+        <v>250000</v>
       </c>
       <c r="G8" s="22">
-        <v>250000</v>
-      </c>
-      <c r="H8" s="22">
         <v>66666</v>
       </c>
+      <c r="H8">
+        <v>70.099999999999994</v>
+      </c>
       <c r="I8">
-        <v>70.099999999999994</v>
+        <v>193.3</v>
       </c>
       <c r="J8">
-        <v>193.3</v>
+        <v>1304</v>
       </c>
       <c r="K8">
-        <v>1304</v>
-      </c>
-      <c r="L8">
         <v>1385</v>
       </c>
+      <c r="L8" s="22">
+        <f>G8/(H8/100)</f>
+        <v>95101.283880171191</v>
+      </c>
       <c r="M8" s="22">
-        <f>H8/(I8/100)</f>
-        <v>95101.283880171191</v>
+        <f>G8/(I8/100)</f>
+        <v>34488.360062079671</v>
       </c>
       <c r="N8" s="22">
-        <f>H8/(J8/100)</f>
-        <v>34488.360062079671</v>
-      </c>
-      <c r="O8" s="22">
-        <f>H8/D8</f>
+        <f>G8/D8</f>
         <v>16666.5</v>
       </c>
     </row>
-    <row r="9" spans="2:15" hidden="1">
+    <row r="9" spans="2:14" hidden="1">
       <c r="B9" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9">
         <v>4</v>
       </c>
-      <c r="E9">
-        <v>1000</v>
+      <c r="E9" s="22">
+        <v>1000000</v>
       </c>
       <c r="F9" s="22">
-        <v>1000000</v>
+        <v>250000</v>
       </c>
       <c r="G9" s="22">
-        <v>250000</v>
-      </c>
-      <c r="H9" s="22">
         <v>66666</v>
       </c>
+      <c r="H9">
+        <v>97.6</v>
+      </c>
       <c r="I9">
-        <v>97.6</v>
+        <v>189.9</v>
       </c>
       <c r="J9">
-        <v>189.9</v>
+        <v>1785</v>
       </c>
       <c r="K9">
-        <v>1785</v>
-      </c>
-      <c r="L9">
         <v>1913</v>
       </c>
+      <c r="L9" s="22">
+        <f>G9/(H9/100)</f>
+        <v>68305.327868852459</v>
+      </c>
       <c r="M9" s="22">
-        <f>H9/(I9/100)</f>
-        <v>68305.327868852459</v>
+        <f>G9/(I9/100)</f>
+        <v>35105.845181674566</v>
       </c>
       <c r="N9" s="22">
-        <f>H9/(J9/100)</f>
-        <v>35105.845181674566</v>
-      </c>
-      <c r="O9" s="22">
-        <f>H9/D9</f>
+        <f>G9/D9</f>
         <v>16666.5</v>
       </c>
     </row>
-    <row r="10" spans="2:15">
+    <row r="10" spans="2:14">
       <c r="B10" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10">
         <v>5</v>
       </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>35000</v>
+      <c r="E10" s="22">
+        <v>1000000</v>
       </c>
       <c r="F10" s="22">
-        <v>1000000</v>
+        <v>200000</v>
       </c>
       <c r="G10" s="22">
-        <v>200000</v>
-      </c>
-      <c r="H10" s="22">
         <v>66666</v>
       </c>
+      <c r="H10">
+        <v>73.3</v>
+      </c>
       <c r="I10">
-        <v>73.3</v>
+        <v>284.7</v>
       </c>
       <c r="J10">
-        <v>284.7</v>
+        <v>1562</v>
       </c>
       <c r="K10">
-        <v>1562</v>
-      </c>
-      <c r="L10">
         <v>1663</v>
       </c>
+      <c r="L10" s="22">
+        <f>G10/(H10/100)</f>
+        <v>90949.522510231924</v>
+      </c>
       <c r="M10" s="22">
-        <f>H10/(I10/100)</f>
-        <v>90949.522510231924</v>
+        <f>G10/(I10/100)</f>
+        <v>23416.22760800843</v>
       </c>
       <c r="N10" s="22">
-        <f>H10/(J10/100)</f>
-        <v>23416.22760800843</v>
-      </c>
-      <c r="O10" s="22">
-        <f>H10/D10</f>
+        <f>G10/D10</f>
         <v>13333.2</v>
       </c>
     </row>
-    <row r="12" spans="2:15">
-      <c r="B12" s="21" t="s">
+    <row r="12" spans="2:14">
+      <c r="B12" s="21"/>
+    </row>
+    <row r="13" spans="2:14">
+      <c r="B13" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14">
+      <c r="B14" s="21" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15">
-      <c r="B13" s="21" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3252E9FD-B0D5-4A5E-93CF-83CC5206BFAB}">
+  <dimension ref="B2:L10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12">
+      <c r="B2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="21">
+        <v>15</v>
+      </c>
+      <c r="D3" s="22">
+        <v>62500</v>
+      </c>
+      <c r="E3" s="22">
+        <v>500000</v>
+      </c>
+      <c r="F3">
+        <v>1.7</v>
+      </c>
+      <c r="G3">
+        <v>3.47</v>
+      </c>
+      <c r="I3">
+        <v>4450</v>
+      </c>
+      <c r="J3">
+        <v>8</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3" s="22">
+        <v>35600</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4" s="22">
+        <v>93750</v>
+      </c>
+      <c r="E4" s="22">
+        <v>750000</v>
+      </c>
+      <c r="F4">
+        <v>2.7</v>
+      </c>
+      <c r="G4">
+        <v>5.67</v>
+      </c>
+      <c r="I4">
+        <v>8900</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+      <c r="L4" s="22">
+        <v>35600</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5" s="22">
+        <v>125000</v>
+      </c>
+      <c r="E5" s="22">
+        <v>1000000</v>
+      </c>
+      <c r="F5">
+        <v>3.03</v>
+      </c>
+      <c r="G5">
+        <v>5.62</v>
+      </c>
+      <c r="I5" s="22">
+        <v>16500</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5" s="22">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6">
+        <v>3.06</v>
+      </c>
+      <c r="G6">
+        <v>5.62</v>
+      </c>
+      <c r="I6" s="22">
+        <v>29500</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6" s="22">
+        <v>29500</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="I7">
+        <v>5250</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>8</v>
+      </c>
+      <c r="L7" s="22">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="B9" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="B10" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>